<commit_message>
salvando dados do extrato e categorizando
</commit_message>
<xml_diff>
--- a/app/static/docs_repository/extrato/extrato1.xlsx
+++ b/app/static/docs_repository/extrato/extrato1.xlsx
@@ -11,11 +11,11 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="HTML_1" vbProcedure="false">$A$1:$H$30</definedName>
-    <definedName function="false" hidden="false" name="HTML_2" vbProcedure="false">$A$1:$A$1</definedName>
-    <definedName function="false" hidden="false" name="HTML_3" vbProcedure="false">$A$10:$A$10</definedName>
-    <definedName function="false" hidden="false" name="HTML_all" vbProcedure="false">$A$1:$H$30</definedName>
-    <definedName function="false" hidden="false" name="HTML_tables" vbProcedure="false">$A$1:$A$1</definedName>
+    <definedName function="false" hidden="false" name="HTML_1" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" name="HTML_2" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" name="HTML_3" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" name="HTML_all" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" name="HTML_tables" vbProcedure="false">#REF!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t xml:space="preserve">Nome:</t>
   </si>
@@ -68,36 +68,24 @@
     <t xml:space="preserve">Saldo (R$)</t>
   </si>
   <si>
-    <t xml:space="preserve">28/11  </t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">SALDO ANTERIOR</t>
   </si>
   <si>
-    <t xml:space="preserve">29/11  </t>
-  </si>
-  <si>
     <t xml:space="preserve">TEC DEPOSITO DINHEIRO</t>
   </si>
   <si>
     <t xml:space="preserve">SALDO DO DIA</t>
   </si>
   <si>
-    <t xml:space="preserve">30/11  </t>
-  </si>
-  <si>
     <t xml:space="preserve">TED 237.3396MAZZ SERV CO</t>
   </si>
   <si>
     <t xml:space="preserve">ITAUCARD-2302-8990-PGMIN</t>
   </si>
   <si>
-    <t xml:space="preserve">01/12  </t>
-  </si>
-  <si>
     <t xml:space="preserve">LIS/JUROS</t>
   </si>
   <si>
@@ -114,9 +102,6 @@
   </si>
   <si>
     <t xml:space="preserve">EST LIS/JUROS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02/12  </t>
   </si>
   <si>
     <t xml:space="preserve">RSHOP-A C SALGADO-02/12</t>
@@ -132,9 +117,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -211,7 +198,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -229,6 +216,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -256,12 +251,14 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -402,324 +399,324 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
+      <c r="B12" s="5" t="n">
+        <v>43067</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2" t="n">
+      <c r="F12" s="6"/>
+      <c r="G12" s="6" t="n">
         <v>-726.91</v>
       </c>
       <c r="H12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
-      <c r="B13" s="2" t="s">
-        <v>16</v>
+      <c r="B13" s="5" t="n">
+        <v>43068</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="F13" s="6" t="n">
         <v>60</v>
       </c>
-      <c r="G13" s="2"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
-      <c r="B14" s="2" t="s">
-        <v>16</v>
+      <c r="B14" s="5" t="n">
+        <v>43068</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6" t="n">
         <v>-666.91</v>
       </c>
       <c r="H14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
-        <v>19</v>
+      <c r="B15" s="5" t="n">
+        <v>43069</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="F15" s="6" t="n">
         <v>641.67</v>
       </c>
-      <c r="G15" s="2"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
-      <c r="B16" s="2" t="s">
-        <v>19</v>
+      <c r="B16" s="5" t="n">
+        <v>43069</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="F16" s="6" t="n">
         <v>-116.3</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
-      <c r="B17" s="2" t="s">
-        <v>19</v>
+      <c r="B17" s="5" t="n">
+        <v>43069</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6" t="n">
         <v>-141.54</v>
       </c>
       <c r="H17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
-      <c r="B18" s="3" t="s">
-        <v>22</v>
+      <c r="B18" s="5" t="n">
+        <v>43070</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="F18" s="6" t="n">
         <v>-46.88</v>
       </c>
-      <c r="G18" s="2"/>
+      <c r="G18" s="6"/>
       <c r="H18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
-      <c r="B19" s="3" t="s">
-        <v>22</v>
+      <c r="B19" s="5" t="n">
+        <v>43070</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="F19" s="6" t="n">
         <v>-5.6</v>
       </c>
-      <c r="G19" s="2"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
-      <c r="B20" s="3" t="s">
-        <v>22</v>
+      <c r="B20" s="5" t="n">
+        <v>43070</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="F20" s="6" t="n">
         <v>-50</v>
       </c>
-      <c r="G20" s="2"/>
+      <c r="G20" s="6"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
-      <c r="B21" s="3" t="s">
-        <v>22</v>
+      <c r="B21" s="5" t="n">
+        <v>43070</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="F21" s="6" t="n">
         <v>-15</v>
       </c>
-      <c r="G21" s="2"/>
+      <c r="G21" s="6"/>
       <c r="H21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
-      <c r="B22" s="3" t="s">
-        <v>22</v>
+      <c r="B22" s="5" t="n">
+        <v>43070</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="F22" s="6" t="n">
         <v>-47.65</v>
       </c>
-      <c r="G22" s="2"/>
+      <c r="G22" s="6"/>
       <c r="H22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
-      <c r="B23" s="3" t="s">
-        <v>22</v>
+      <c r="B23" s="5" t="n">
+        <v>43070</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="F23" s="6" t="n">
         <v>-4.64</v>
       </c>
-      <c r="G23" s="2"/>
+      <c r="G23" s="6"/>
       <c r="H23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
-      <c r="B24" s="3" t="s">
-        <v>22</v>
+      <c r="B24" s="5" t="n">
+        <v>43070</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F24" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="F24" s="6" t="n">
         <v>46.88</v>
       </c>
-      <c r="G24" s="2"/>
+      <c r="G24" s="6"/>
       <c r="H24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
-      <c r="B25" s="3" t="s">
-        <v>22</v>
+      <c r="B25" s="5" t="n">
+        <v>43070</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6" t="n">
         <v>-264.43</v>
       </c>
       <c r="H25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
-      <c r="B26" s="3" t="s">
-        <v>29</v>
+      <c r="B26" s="5" t="n">
+        <v>43071</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="F26" s="6" t="n">
         <v>-8.5</v>
       </c>
-      <c r="G26" s="2"/>
+      <c r="G26" s="6"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
-      <c r="B27" s="3" t="s">
-        <v>29</v>
+      <c r="B27" s="5" t="n">
+        <v>43071</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F27" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="F27" s="6" t="n">
         <v>-15</v>
       </c>
-      <c r="G27" s="2"/>
+      <c r="G27" s="6"/>
       <c r="H27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
-      <c r="B28" s="3" t="s">
-        <v>29</v>
+      <c r="B28" s="5" t="n">
+        <v>43071</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="F28" s="6" t="n">
         <v>-16.97</v>
       </c>
-      <c r="G28" s="2"/>
+      <c r="G28" s="6"/>
       <c r="H28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
-      <c r="B29" s="3" t="s">
-        <v>29</v>
+      <c r="B29" s="5" t="n">
+        <v>43071</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6" t="n">
         <v>-304.9</v>
       </c>
       <c r="H29" s="2"/>

</xml_diff>